<commit_message>
prepare dataset for commentary spotting experiment
</commit_message>
<xml_diff>
--- a/annotation_tool/subcategory_annotation_sheet.xlsx
+++ b/annotation_tool/subcategory_annotation_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heste/workspace/soccernet/sn-script/annotation_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DDDED5-342E-B94B-8CF6-DCA26A4C3070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA58CF5-A135-2D46-8289-01A48E6C6EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10560" yWindow="-28300" windowWidth="51200" windowHeight="14160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10720" yWindow="-28300" windowWidth="51200" windowHeight="14160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="93_1_moriy" sheetId="12" r:id="rId1"/>
@@ -6411,7 +6411,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I80" sqref="I80"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>

</xml_diff>